<commit_message>
Made a few changes in master EDAbio.R and changed t baselinepredctivemodel branch
</commit_message>
<xml_diff>
--- a/Covariate_dictionary.xlsx
+++ b/Covariate_dictionary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bbodinie/Dropbox/Teaching/Translational_Data_Science/Project_19-20/Data/UK_Biobank/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luischavesrodriguez/OneDrive - Imperial College London/MScHDA/Term2/TDS/Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B75DC898-640E-114C-BA37-2ABB20305D86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12520" yWindow="460" windowWidth="20960" windowHeight="19740" xr2:uid="{9350B2D7-2A70-2141-8C51-D24CA1FF3769}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{9350B2D7-2A70-2141-8C51-D24CA1FF3769}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
may have done some changes in my compi
</commit_message>
<xml_diff>
--- a/Covariate_dictionary.xlsx
+++ b/Covariate_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luischavesrodriguez/OneDrive - Imperial College London/MScHDA/Term2/TDS/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/lc5415_ic_ac_uk/Documents/MScHDA/Term2/TDS/Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B75DC898-640E-114C-BA37-2ABB20305D86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{B75DC898-640E-114C-BA37-2ABB20305D86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CD2244D7-9F29-D648-8CFF-09EF7F3E2B91}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{9350B2D7-2A70-2141-8C51-D24CA1FF3769}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16000" xr2:uid="{9350B2D7-2A70-2141-8C51-D24CA1FF3769}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,9 +68,6 @@
     <t>age_cl</t>
   </si>
   <si>
-    <t>age class</t>
-  </si>
-  <si>
     <t>stop</t>
   </si>
   <si>
@@ -252,6 +249,9 @@
   </si>
   <si>
     <t>Age at death or end of follow up</t>
+  </si>
+  <si>
+    <t>Age class</t>
   </si>
 </sst>
 </file>
@@ -605,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECF67AD2-C4BD-824D-8E51-127B6E2D700E}">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection sqref="A1:B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -628,7 +628,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -644,7 +644,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -668,188 +668,188 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
         <v>16</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
         <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
         <v>21</v>
-      </c>
-      <c r="B14" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
         <v>23</v>
-      </c>
-      <c r="B15" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
         <v>25</v>
-      </c>
-      <c r="B16" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
         <v>27</v>
-      </c>
-      <c r="B17" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
         <v>29</v>
-      </c>
-      <c r="B18" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" t="s">
         <v>32</v>
-      </c>
-      <c r="B20" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" t="s">
         <v>35</v>
-      </c>
-      <c r="B21" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" t="s">
         <v>37</v>
-      </c>
-      <c r="B22" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B30" t="s">
         <v>4</v>
@@ -857,15 +857,15 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B32" t="s">
         <v>7</v>
@@ -873,50 +873,50 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" t="s">
         <v>57</v>
-      </c>
-      <c r="B33" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" t="s">
         <v>59</v>
-      </c>
-      <c r="B34" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" t="s">
         <v>61</v>
-      </c>
-      <c r="B35" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" t="s">
         <v>63</v>
-      </c>
-      <c r="B36" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" t="s">
         <v>65</v>
-      </c>
-      <c r="B37" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" t="s">
         <v>67</v>
-      </c>
-      <c r="B38" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>